<commit_message>
added a bunch of small features!
</commit_message>
<xml_diff>
--- a/phrasetest.xlsx
+++ b/phrasetest.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>我</t>
   </si>
@@ -59,16 +59,7 @@
     <t>wǎngshì</t>
   </si>
   <si>
-    <t>past</t>
-  </si>
-  <si>
-    <t>fug</t>
-  </si>
-  <si>
-    <t>fugg</t>
-  </si>
-  <si>
-    <t>This is a test to see how long the definition of fugg can be.</t>
+    <t>To spend time with one's loved ones</t>
   </si>
 </sst>
 </file>
@@ -420,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC72745E-7A98-4E23-9D2F-AC77EBDA8522}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -475,17 +466,6 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>